<commit_message>
Added 13 models of Beyma
</commit_message>
<xml_diff>
--- a/Speaker DB/SpeakerDB (March 2019).xlsx
+++ b/Speaker DB/SpeakerDB (March 2019).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmrplens/Documents/GitHub/LoVE-BASS/Speaker DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D4A073-4442-0D4B-AE65-318074FAF07B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E564DC21-AA38-D94A-BF77-59650501E1C1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="256">
   <si>
     <t>Name</t>
   </si>
@@ -763,6 +763,45 @@
   </si>
   <si>
     <t>B&amp;C Speakers 8PS21_8</t>
+  </si>
+  <si>
+    <t>Beyma 10LW30_N</t>
+  </si>
+  <si>
+    <t>Beyma 12LW30_N</t>
+  </si>
+  <si>
+    <t>Beyma 12WR400</t>
+  </si>
+  <si>
+    <t>Beyma 15LEX1600Nd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beyma 15LW30 </t>
+  </si>
+  <si>
+    <t>Beyma 15SW1300Nd</t>
+  </si>
+  <si>
+    <t>Beyma 6MI100</t>
+  </si>
+  <si>
+    <t>Beyma 6MI90</t>
+  </si>
+  <si>
+    <t>Beyma 6P200Nd</t>
+  </si>
+  <si>
+    <t>Beyma 8LW30</t>
+  </si>
+  <si>
+    <t>Beyma 8WOOFER_P V2</t>
+  </si>
+  <si>
+    <t>Beyma 8CM_B</t>
+  </si>
+  <si>
+    <t>Beyma 605Nd</t>
   </si>
 </sst>
 </file>
@@ -1427,9 +1466,9 @@
   <dimension ref="A1:Q493"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2080" topLeftCell="A3" activePane="bottomLeft"/>
+      <pane ySplit="2080" topLeftCell="A135" activePane="bottomLeft"/>
       <selection sqref="A1:J1048576"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomLeft" activeCell="L158" sqref="L158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6520,217 +6559,217 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A145" s="6" t="s">
-        <v>58</v>
+        <v>243</v>
       </c>
       <c r="B145" s="7">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C145" s="7">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="D145" s="7">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="E145" s="7">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="F145" s="7">
-        <v>350</v>
+        <v>350.00000000000006</v>
       </c>
       <c r="G145" s="7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H145" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I145" s="7">
         <v>1</v>
       </c>
       <c r="J145" s="5">
-        <v>500</v>
+        <v>450</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A146" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B146" s="7">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C146" s="7">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="D146" s="7">
-        <v>3.8</v>
+        <v>7.5</v>
       </c>
       <c r="E146" s="7">
-        <v>0.24</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F146" s="7">
         <v>350</v>
       </c>
       <c r="G146" s="7">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H146" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I146" s="7">
         <v>1</v>
       </c>
       <c r="J146" s="5">
-        <v>700</v>
+        <v>500</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A147" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B147" s="7">
-        <v>260</v>
+        <v>63</v>
       </c>
       <c r="C147" s="7">
-        <v>5.8</v>
+        <v>5.2</v>
       </c>
       <c r="D147" s="7">
-        <v>22</v>
+        <v>3.8</v>
       </c>
       <c r="E147" s="7">
-        <v>0.45</v>
+        <v>0.24</v>
       </c>
       <c r="F147" s="7">
-        <v>380</v>
+        <v>350</v>
       </c>
       <c r="G147" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H147" s="7">
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="I147" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J147" s="5">
-        <v>400</v>
+        <v>700</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A148" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B148" s="7">
-        <v>70</v>
+        <v>260</v>
       </c>
       <c r="C148" s="7">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
       <c r="D148" s="7">
-        <v>10.1</v>
+        <v>22</v>
       </c>
       <c r="E148" s="7">
-        <v>0.38</v>
+        <v>0.45</v>
       </c>
       <c r="F148" s="7">
-        <v>350</v>
+        <v>380</v>
       </c>
       <c r="G148" s="7">
-        <v>18.8</v>
+        <v>2</v>
       </c>
       <c r="H148" s="7">
-        <v>8</v>
+        <v>3.5</v>
       </c>
       <c r="I148" s="7">
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="J148" s="5">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A149" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B149" s="7">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C149" s="7">
-        <v>6.3</v>
+        <v>5.7</v>
       </c>
       <c r="D149" s="7">
-        <v>6.6</v>
+        <v>10.1</v>
       </c>
       <c r="E149" s="7">
-        <v>0.22</v>
+        <v>0.38</v>
       </c>
       <c r="F149" s="7">
-        <v>380</v>
+        <v>350</v>
       </c>
       <c r="G149" s="7">
-        <v>54</v>
+        <v>18.8</v>
       </c>
       <c r="H149" s="7">
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="I149" s="7">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J149" s="5">
-        <v>350</v>
+        <v>500</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A150" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B150" s="7">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C150" s="7">
-        <v>6.1</v>
+        <v>6.3</v>
       </c>
       <c r="D150" s="7">
-        <v>3.9</v>
+        <v>6.6</v>
       </c>
       <c r="E150" s="7">
-        <v>0.35</v>
+        <v>0.22</v>
       </c>
       <c r="F150" s="7">
+        <v>380</v>
+      </c>
+      <c r="G150" s="7">
+        <v>54</v>
+      </c>
+      <c r="H150" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="I150" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J150" s="5">
         <v>350</v>
-      </c>
-      <c r="G150" s="7">
-        <v>50.9</v>
-      </c>
-      <c r="H150" s="7">
-        <v>6</v>
-      </c>
-      <c r="I150" s="7">
-        <v>1</v>
-      </c>
-      <c r="J150" s="5">
-        <v>300</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A151" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B151" s="7">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C151" s="7">
         <v>6.1</v>
       </c>
       <c r="D151" s="7">
-        <v>5.5</v>
+        <v>3.9</v>
       </c>
       <c r="E151" s="7">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="F151" s="7">
         <v>350</v>
       </c>
       <c r="G151" s="7">
-        <v>39.299999999999997</v>
+        <v>50.9</v>
       </c>
       <c r="H151" s="7">
         <v>6</v>
@@ -6744,223 +6783,223 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A152" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B152" s="7">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C152" s="7">
-        <v>5.6</v>
+        <v>6.1</v>
       </c>
       <c r="D152" s="7">
-        <v>4.4400000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="E152" s="7">
-        <v>0.56000000000000005</v>
+        <v>0.4</v>
       </c>
       <c r="F152" s="7">
-        <v>540</v>
+        <v>350</v>
       </c>
       <c r="G152" s="7">
-        <v>142</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="H152" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I152" s="7">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="J152" s="5">
-        <v>125</v>
+        <v>300</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A153" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B153" s="7">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C153" s="7">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="D153" s="7">
-        <v>3.9</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="E153" s="7">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F153" s="7">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="G153" s="7">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="H153" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I153" s="7">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="J153" s="5">
-        <v>320</v>
+        <v>125</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A154" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B154" s="7">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C154" s="7">
         <v>6</v>
       </c>
       <c r="D154" s="7">
-        <v>11.6</v>
+        <v>3.9</v>
       </c>
       <c r="E154" s="7">
-        <v>0.3</v>
+        <v>0.54</v>
       </c>
       <c r="F154" s="7">
         <v>530</v>
       </c>
       <c r="G154" s="7">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H154" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I154" s="7">
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="J154" s="5">
-        <v>500</v>
+        <v>320</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A155" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B155" s="7">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="C155" s="7">
-        <v>6.2</v>
+        <v>6</v>
       </c>
       <c r="D155" s="7">
-        <v>14.8</v>
+        <v>11.6</v>
       </c>
       <c r="E155" s="7">
-        <v>1.26</v>
+        <v>0.3</v>
       </c>
       <c r="F155" s="7">
         <v>530</v>
       </c>
       <c r="G155" s="7">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="H155" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I155" s="7">
-        <v>0.6</v>
+        <v>2.1</v>
       </c>
       <c r="J155" s="5">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A156" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B156" s="7">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C156" s="7">
-        <v>5.0999999999999996</v>
+        <v>6.2</v>
       </c>
       <c r="D156" s="7">
-        <v>15.3</v>
+        <v>14.8</v>
       </c>
       <c r="E156" s="7">
-        <v>0.4</v>
+        <v>1.26</v>
       </c>
       <c r="F156" s="7">
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="G156" s="7">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H156" s="7">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I156" s="7">
-        <v>2.1</v>
+        <v>0.6</v>
       </c>
       <c r="J156" s="5">
-        <v>700</v>
+        <v>250</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A157" s="6" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
       <c r="B157" s="7">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C157" s="7">
-        <v>5.5</v>
+        <v>6.3</v>
       </c>
       <c r="D157" s="7">
-        <v>8.6</v>
+        <v>3.8</v>
       </c>
       <c r="E157" s="7">
-        <v>0.39</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F157" s="7">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="G157" s="7">
-        <v>54.9</v>
+        <v>84</v>
       </c>
       <c r="H157" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I157" s="7">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J157" s="5">
-        <v>500</v>
+        <v>450</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A158" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B158" s="7">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C158" s="7">
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D158" s="7">
-        <v>4.0999999999999996</v>
+        <v>15.3</v>
       </c>
       <c r="E158" s="7">
-        <v>0.26</v>
+        <v>0.4</v>
       </c>
       <c r="F158" s="7">
         <v>550</v>
       </c>
       <c r="G158" s="7">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="H158" s="7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I158" s="7">
-        <v>1</v>
+        <v>2.1</v>
       </c>
       <c r="J158" s="5">
         <v>700</v>
@@ -6968,31 +7007,31 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A159" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B159" s="7">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C159" s="7">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="D159" s="7">
-        <v>7.8</v>
+        <v>8.6</v>
       </c>
       <c r="E159" s="7">
-        <v>0.44</v>
+        <v>0.39</v>
       </c>
       <c r="F159" s="7">
         <v>550</v>
       </c>
       <c r="G159" s="7">
-        <v>44</v>
+        <v>54.9</v>
       </c>
       <c r="H159" s="7">
         <v>8</v>
       </c>
       <c r="I159" s="7">
-        <v>1.1000000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="J159" s="5">
         <v>500</v>
@@ -7000,380 +7039,380 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A160" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B160" s="7">
+        <v>51</v>
+      </c>
+      <c r="C160" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="D160" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E160" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="F160" s="7">
+        <v>550</v>
+      </c>
+      <c r="G160" s="7">
         <v>58</v>
       </c>
-      <c r="C160" s="7">
-        <v>6.3</v>
-      </c>
-      <c r="D160" s="7">
-        <v>5.54</v>
-      </c>
-      <c r="E160" s="7">
-        <v>0.23</v>
-      </c>
-      <c r="F160" s="7">
-        <v>530</v>
-      </c>
-      <c r="G160" s="7">
-        <v>64</v>
-      </c>
       <c r="H160" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I160" s="7">
         <v>1</v>
       </c>
       <c r="J160" s="5">
-        <v>450</v>
+        <v>700</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A161" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B161" s="7">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C161" s="7">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="D161" s="7">
-        <v>7.89</v>
+        <v>7.8</v>
       </c>
       <c r="E161" s="7">
-        <v>0.27</v>
+        <v>0.44</v>
       </c>
       <c r="F161" s="7">
         <v>550</v>
       </c>
       <c r="G161" s="7">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H161" s="7">
         <v>8</v>
       </c>
       <c r="I161" s="7">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J161" s="5">
-        <v>900</v>
+        <v>500</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A162" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B162" s="7">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C162" s="7">
-        <v>5</v>
+        <v>6.3</v>
       </c>
       <c r="D162" s="7">
-        <v>6.5</v>
+        <v>5.54</v>
       </c>
       <c r="E162" s="7">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="F162" s="7">
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="G162" s="7">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H162" s="7">
-        <v>7.5</v>
+        <v>2</v>
       </c>
       <c r="I162" s="7">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="J162" s="5">
-        <v>700</v>
+        <v>450</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A163" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B163" s="7">
         <v>47</v>
       </c>
       <c r="C163" s="7">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D163" s="7">
-        <v>5.2</v>
+        <v>7.89</v>
       </c>
       <c r="E163" s="7">
-        <v>0.2</v>
+        <v>0.27</v>
       </c>
       <c r="F163" s="7">
         <v>550</v>
       </c>
       <c r="G163" s="7">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="H163" s="7">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="I163" s="7">
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="J163" s="5">
-        <v>700</v>
+        <v>900</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A164" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B164" s="7">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C164" s="7">
-        <v>4.9000000000000004</v>
+        <v>5</v>
       </c>
       <c r="D164" s="7">
-        <v>12.07</v>
+        <v>6.5</v>
       </c>
       <c r="E164" s="7">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
       <c r="F164" s="7">
         <v>550</v>
       </c>
       <c r="G164" s="7">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H164" s="7">
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="I164" s="7">
-        <v>3.25</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J164" s="5">
-        <v>1200</v>
+        <v>700</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A165" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B165" s="7">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C165" s="7">
-        <v>5.6</v>
+        <v>5</v>
       </c>
       <c r="D165" s="7">
-        <v>7.7</v>
+        <v>5.2</v>
       </c>
       <c r="E165" s="7">
-        <v>0.32</v>
+        <v>0.2</v>
       </c>
       <c r="F165" s="7">
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="G165" s="7">
-        <v>77.900000000000006</v>
+        <v>65</v>
       </c>
       <c r="H165" s="7">
-        <v>6.3</v>
+        <v>7.5</v>
       </c>
       <c r="I165" s="7">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="J165" s="5">
-        <v>400</v>
+        <v>700</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A166" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B166" s="7">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C166" s="7">
-        <v>6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D166" s="7">
-        <v>4.0999999999999996</v>
+        <v>12.07</v>
       </c>
       <c r="E166" s="7">
-        <v>0.55000000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="F166" s="7">
-        <v>880</v>
+        <v>550</v>
       </c>
       <c r="G166" s="7">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="H166" s="7">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I166" s="7">
-        <v>1.2</v>
+        <v>3.25</v>
       </c>
       <c r="J166" s="5">
-        <v>350</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A167" s="6" t="s">
-        <v>80</v>
+        <v>245</v>
       </c>
       <c r="B167" s="7">
         <v>42</v>
       </c>
       <c r="C167" s="7">
-        <v>5.0999999999999996</v>
+        <v>5.8</v>
       </c>
       <c r="D167" s="7">
-        <v>21.2</v>
+        <v>5.6</v>
       </c>
       <c r="E167" s="7">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="F167" s="7">
-        <v>910</v>
+        <v>530</v>
       </c>
       <c r="G167" s="7">
-        <v>105</v>
+        <v>91.1</v>
       </c>
       <c r="H167" s="7">
-        <v>9</v>
+        <v>6.3</v>
       </c>
       <c r="I167" s="7">
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="J167" s="5">
-        <v>700</v>
+        <v>400</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A168" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B168" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C168" s="7">
-        <v>5.7</v>
+        <v>5.6</v>
       </c>
       <c r="D168" s="7">
-        <v>8</v>
+        <v>7.7</v>
       </c>
       <c r="E168" s="7">
-        <v>0.49</v>
+        <v>0.32</v>
       </c>
       <c r="F168" s="7">
-        <v>880</v>
+        <v>530</v>
       </c>
       <c r="G168" s="7">
-        <v>131.5</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="H168" s="7">
-        <v>8</v>
+        <v>6.3</v>
       </c>
       <c r="I168" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="J168" s="5">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A169" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B169" s="7">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C169" s="7">
         <v>6</v>
       </c>
       <c r="D169" s="7">
-        <v>5.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E169" s="7">
-        <v>0.4</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F169" s="7">
         <v>880</v>
       </c>
       <c r="G169" s="7">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="H169" s="7">
-        <v>9.8000000000000007</v>
+        <v>7</v>
       </c>
       <c r="I169" s="7">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="J169" s="5">
-        <v>700</v>
+        <v>350</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A170" s="6" t="s">
-        <v>83</v>
+        <v>246</v>
       </c>
       <c r="B170" s="7">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C170" s="7">
-        <v>5.2</v>
+        <v>5.5</v>
       </c>
       <c r="D170" s="7">
-        <v>3.6</v>
+        <v>6.6</v>
       </c>
       <c r="E170" s="7">
-        <v>0.34</v>
+        <v>0.38</v>
       </c>
       <c r="F170" s="7">
         <v>880</v>
       </c>
       <c r="G170" s="7">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="H170" s="7">
-        <v>7</v>
+        <v>14.5</v>
       </c>
       <c r="I170" s="7">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="J170" s="5">
-        <v>700</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A171" s="6" t="s">
-        <v>84</v>
+        <v>247</v>
       </c>
       <c r="B171" s="7">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C171" s="7">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
       <c r="D171" s="7">
-        <v>7.8</v>
+        <v>4.5</v>
       </c>
       <c r="E171" s="7">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="F171" s="7">
         <v>880</v>
       </c>
       <c r="G171" s="7">
-        <v>133.5</v>
+        <v>251</v>
       </c>
       <c r="H171" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I171" s="7">
         <v>1.1000000000000001</v>
@@ -7384,1149 +7423,1149 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A172" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B172" s="7">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C172" s="7">
-        <v>6.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D172" s="7">
-        <v>6.3</v>
+        <v>21.2</v>
       </c>
       <c r="E172" s="7">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="F172" s="7">
-        <v>880</v>
+        <v>910</v>
       </c>
       <c r="G172" s="7">
-        <v>264</v>
+        <v>105</v>
       </c>
       <c r="H172" s="7">
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="I172" s="7">
-        <v>1</v>
+        <v>2.1</v>
       </c>
       <c r="J172" s="5">
-        <v>450</v>
+        <v>700</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A173" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B173" s="7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C173" s="7">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="D173" s="7">
-        <v>5.9</v>
+        <v>8</v>
       </c>
       <c r="E173" s="7">
-        <v>0.31</v>
+        <v>0.49</v>
       </c>
       <c r="F173" s="7">
-        <v>855</v>
+        <v>880</v>
       </c>
       <c r="G173" s="7">
-        <v>80.7</v>
+        <v>131.5</v>
       </c>
       <c r="H173" s="7">
         <v>8</v>
       </c>
       <c r="I173" s="7">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J173" s="5">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A174" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B174" s="7">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C174" s="7">
+        <v>6</v>
+      </c>
+      <c r="D174" s="7">
         <v>5.3</v>
       </c>
-      <c r="D174" s="7">
-        <v>5.5</v>
-      </c>
       <c r="E174" s="7">
-        <v>0.19</v>
+        <v>0.4</v>
       </c>
       <c r="F174" s="7">
         <v>880</v>
       </c>
       <c r="G174" s="7">
-        <v>305</v>
+        <v>148</v>
       </c>
       <c r="H174" s="7">
-        <v>7.5</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I174" s="7">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="J174" s="5">
-        <v>800</v>
+        <v>700</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A175" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B175" s="7">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C175" s="7">
-        <v>5.0999999999999996</v>
+        <v>5.2</v>
       </c>
       <c r="D175" s="7">
-        <v>5.0999999999999996</v>
+        <v>3.6</v>
       </c>
       <c r="E175" s="7">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="F175" s="7">
         <v>880</v>
       </c>
       <c r="G175" s="7">
-        <v>184</v>
+        <v>105</v>
       </c>
       <c r="H175" s="7">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="I175" s="7">
         <v>0.8</v>
       </c>
       <c r="J175" s="5">
-        <v>800</v>
+        <v>700</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A176" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B176" s="7">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C176" s="7">
-        <v>5.5</v>
+        <v>5.8</v>
       </c>
       <c r="D176" s="7">
-        <v>8.1999999999999993</v>
+        <v>7.8</v>
       </c>
       <c r="E176" s="7">
-        <v>0.32</v>
+        <v>0.5</v>
       </c>
       <c r="F176" s="7">
         <v>880</v>
       </c>
       <c r="G176" s="7">
-        <v>224</v>
+        <v>133.5</v>
       </c>
       <c r="H176" s="7">
-        <v>6.3</v>
+        <v>8</v>
       </c>
       <c r="I176" s="7">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J176" s="5">
-        <v>400</v>
+        <v>500</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A177" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B177" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C177" s="7">
-        <v>5.6</v>
+        <v>6.2</v>
       </c>
       <c r="D177" s="7">
-        <v>9.1</v>
+        <v>6.3</v>
       </c>
       <c r="E177" s="7">
-        <v>0.34</v>
+        <v>0.3</v>
       </c>
       <c r="F177" s="7">
         <v>880</v>
       </c>
       <c r="G177" s="7">
-        <v>233</v>
+        <v>264</v>
       </c>
       <c r="H177" s="7">
-        <v>6.3</v>
+        <v>4.5</v>
       </c>
       <c r="I177" s="7">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="J177" s="5">
-        <v>400</v>
+        <v>450</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A178" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B178" s="7">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C178" s="7">
-        <v>5.6</v>
+        <v>5.2</v>
       </c>
       <c r="D178" s="7">
-        <v>7</v>
+        <v>5.9</v>
       </c>
       <c r="E178" s="7">
-        <v>0.42</v>
+        <v>0.31</v>
       </c>
       <c r="F178" s="7">
-        <v>1320</v>
+        <v>855</v>
       </c>
       <c r="G178" s="7">
-        <v>290</v>
+        <v>80.7</v>
       </c>
       <c r="H178" s="7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I178" s="7">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="J178" s="5">
-        <v>900</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A179" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B179" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C179" s="7">
-        <v>5.8</v>
+        <v>5.3</v>
       </c>
       <c r="D179" s="7">
-        <v>11.4</v>
+        <v>5.5</v>
       </c>
       <c r="E179" s="7">
-        <v>0.45</v>
+        <v>0.19</v>
       </c>
       <c r="F179" s="7">
-        <v>1255</v>
+        <v>880</v>
       </c>
       <c r="G179" s="7">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="H179" s="7">
-        <v>14.5</v>
+        <v>7.5</v>
       </c>
       <c r="I179" s="7">
-        <v>1.9</v>
+        <v>1.2</v>
       </c>
       <c r="J179" s="5">
-        <v>1600</v>
+        <v>800</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A180" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B180" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C180" s="7">
         <v>5.0999999999999996</v>
       </c>
       <c r="D180" s="7">
-        <v>15.7</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E180" s="7">
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
       <c r="F180" s="7">
-        <v>1320</v>
+        <v>880</v>
       </c>
       <c r="G180" s="7">
-        <v>236</v>
+        <v>184</v>
       </c>
       <c r="H180" s="7">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="I180" s="7">
-        <v>2.1</v>
+        <v>0.8</v>
       </c>
       <c r="J180" s="5">
-        <v>700</v>
+        <v>800</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A181" s="6" t="s">
-        <v>94</v>
+        <v>248</v>
       </c>
       <c r="B181" s="7">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C181" s="7">
         <v>5.2</v>
       </c>
       <c r="D181" s="7">
-        <v>10.5</v>
+        <v>14.7</v>
       </c>
       <c r="E181" s="7">
-        <v>0.33</v>
+        <v>0.37</v>
       </c>
       <c r="F181" s="7">
-        <v>1250</v>
+        <v>880</v>
       </c>
       <c r="G181" s="7">
-        <v>230</v>
+        <v>89.6</v>
       </c>
       <c r="H181" s="7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I181" s="7">
-        <v>1.75</v>
+        <v>3.45</v>
       </c>
       <c r="J181" s="5">
-        <v>1200</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A182" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B182" s="7">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C182" s="7">
-        <v>5.3</v>
+        <v>5.5</v>
       </c>
       <c r="D182" s="7">
-        <v>10.39</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E182" s="7">
-        <v>0.35</v>
+        <v>0.32</v>
       </c>
       <c r="F182" s="7">
-        <v>1225</v>
+        <v>880</v>
       </c>
       <c r="G182" s="7">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="H182" s="7">
-        <v>9.5</v>
+        <v>6.3</v>
       </c>
       <c r="I182" s="7">
-        <v>2.2999999999999998</v>
+        <v>1</v>
       </c>
       <c r="J182" s="5">
-        <v>1200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A183" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B183" s="7">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C183" s="7">
-        <v>5.0999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="D183" s="7">
-        <v>10.199999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="E183" s="7">
-        <v>0.28000000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="F183" s="7">
-        <v>1255</v>
+        <v>880</v>
       </c>
       <c r="G183" s="7">
-        <v>228.9</v>
+        <v>233</v>
       </c>
       <c r="H183" s="7">
-        <v>10</v>
+        <v>6.3</v>
       </c>
       <c r="I183" s="7">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J183" s="5">
-        <v>1400</v>
+        <v>400</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A184" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B184" s="7">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C184" s="7">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="D184" s="7">
-        <v>8.1999999999999993</v>
+        <v>7</v>
       </c>
       <c r="E184" s="7">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="F184" s="7">
-        <v>1255</v>
+        <v>1320</v>
       </c>
       <c r="G184" s="7">
-        <v>317</v>
+        <v>290</v>
       </c>
       <c r="H184" s="7">
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="I184" s="7">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="J184" s="5">
-        <v>1000</v>
+        <v>900</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A185" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B185" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C185" s="7">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="D185" s="7">
-        <v>4.8</v>
+        <v>11.4</v>
       </c>
       <c r="E185" s="7">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F185" s="7">
         <v>1255</v>
       </c>
       <c r="G185" s="7">
-        <v>372</v>
+        <v>231</v>
       </c>
       <c r="H185" s="7">
-        <v>8.5</v>
+        <v>14.5</v>
       </c>
       <c r="I185" s="7">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="J185" s="5">
-        <v>600</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A186" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B186" s="7">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C186" s="7">
-        <v>5.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D186" s="7">
-        <v>4.4000000000000004</v>
+        <v>15.7</v>
       </c>
       <c r="E186" s="7">
-        <v>0.28999999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="F186" s="7">
-        <v>1734</v>
+        <v>1320</v>
       </c>
       <c r="G186" s="7">
-        <v>394</v>
+        <v>236</v>
       </c>
       <c r="H186" s="7">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I186" s="7">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="J186" s="5">
-        <v>1600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A187" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B187" s="7">
+        <v>33</v>
+      </c>
+      <c r="C187" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="D187" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="E187" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="F187" s="7">
+        <v>1250</v>
+      </c>
+      <c r="G187" s="7">
+        <v>230</v>
+      </c>
+      <c r="H187" s="7">
+        <v>8</v>
+      </c>
+      <c r="I187" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="J187" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A188" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B188" s="7">
+        <v>37</v>
+      </c>
+      <c r="C188" s="7">
+        <v>5.3</v>
+      </c>
+      <c r="D188" s="7">
+        <v>10.39</v>
+      </c>
+      <c r="E188" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="F188" s="7">
+        <v>1225</v>
+      </c>
+      <c r="G188" s="7">
+        <v>198</v>
+      </c>
+      <c r="H188" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="I188" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J188" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A189" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B189" s="7">
+        <v>32</v>
+      </c>
+      <c r="C189" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D189" s="7">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E189" s="7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F189" s="7">
+        <v>1255</v>
+      </c>
+      <c r="G189" s="7">
+        <v>228.9</v>
+      </c>
+      <c r="H189" s="7">
+        <v>10</v>
+      </c>
+      <c r="I189" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="J189" s="5">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A190" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B190" s="7">
+        <v>27</v>
+      </c>
+      <c r="C190" s="7">
+        <v>6</v>
+      </c>
+      <c r="D190" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E190" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="F190" s="7">
+        <v>1255</v>
+      </c>
+      <c r="G190" s="7">
+        <v>317</v>
+      </c>
+      <c r="H190" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="I190" s="7">
+        <v>2</v>
+      </c>
+      <c r="J190" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A191" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B191" s="7">
+        <v>32</v>
+      </c>
+      <c r="C191" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="D191" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="E191" s="7">
+        <v>0.44</v>
+      </c>
+      <c r="F191" s="7">
+        <v>1255</v>
+      </c>
+      <c r="G191" s="7">
+        <v>372</v>
+      </c>
+      <c r="H191" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="I191" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="J191" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A192" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B192" s="7">
+        <v>30</v>
+      </c>
+      <c r="C192" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="D192" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E192" s="7">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F192" s="7">
+        <v>1734</v>
+      </c>
+      <c r="G192" s="7">
+        <v>394</v>
+      </c>
+      <c r="H192" s="7">
+        <v>13</v>
+      </c>
+      <c r="I192" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="J192" s="5">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A193" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B187" s="7">
+      <c r="B193" s="7">
         <v>160</v>
       </c>
-      <c r="C187" s="7">
+      <c r="C193" s="7">
         <v>5.6</v>
       </c>
-      <c r="D187" s="7">
+      <c r="D193" s="7">
         <v>8</v>
       </c>
-      <c r="E187" s="7">
+      <c r="E193" s="7">
         <v>0.52</v>
       </c>
-      <c r="F187" s="7">
+      <c r="F193" s="7">
         <f>0.003*10^4</f>
         <v>30</v>
       </c>
-      <c r="G187" s="7">
+      <c r="G193" s="7">
         <v>0.67</v>
       </c>
-      <c r="H187" s="7">
+      <c r="H193" s="7">
         <v>4.5</v>
       </c>
-      <c r="I187" s="7">
+      <c r="I193" s="7">
         <v>0.25</v>
       </c>
-      <c r="J187" s="5">
+      <c r="J193" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A188" s="6" t="s">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A194" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B188" s="7">
+      <c r="B194" s="7">
         <v>180</v>
       </c>
-      <c r="C188" s="7">
+      <c r="C194" s="7">
         <v>5.5</v>
       </c>
-      <c r="D188" s="7">
+      <c r="D194" s="7">
         <v>9.5</v>
       </c>
-      <c r="E188" s="7">
+      <c r="E194" s="7">
         <v>0.6</v>
       </c>
-      <c r="F188" s="7">
+      <c r="F194" s="7">
         <v>30</v>
       </c>
-      <c r="G188" s="7">
+      <c r="G194" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H188" s="7">
+      <c r="H194" s="7">
         <v>4.5</v>
       </c>
-      <c r="I188" s="7">
+      <c r="I194" s="7">
         <v>0.3</v>
       </c>
-      <c r="J188" s="5">
+      <c r="J194" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A189" s="6" t="s">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A195" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B189" s="7">
+      <c r="B195" s="7">
         <v>92</v>
       </c>
-      <c r="C189" s="7">
+      <c r="C195" s="7">
         <v>6.4</v>
       </c>
-      <c r="D189" s="7">
+      <c r="D195" s="7">
         <v>11.3</v>
       </c>
-      <c r="E189" s="7">
+      <c r="E195" s="7">
         <v>0.96</v>
       </c>
-      <c r="F189" s="7">
+      <c r="F195" s="7">
         <f>0.0055*10^4</f>
         <v>55</v>
       </c>
-      <c r="G189" s="7">
+      <c r="G195" s="7">
         <v>2.8</v>
       </c>
-      <c r="H189" s="7">
+      <c r="H195" s="7">
         <v>3</v>
       </c>
-      <c r="I189" s="7">
+      <c r="I195" s="7">
         <v>0.2</v>
       </c>
-      <c r="J189" s="5">
+      <c r="J195" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A190" s="6" t="s">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A196" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B190" s="7">
+      <c r="B196" s="7">
         <v>94</v>
       </c>
-      <c r="C190" s="7">
+      <c r="C196" s="7">
         <v>6.4</v>
       </c>
-      <c r="D190" s="7">
+      <c r="D196" s="7">
         <v>10.8</v>
       </c>
-      <c r="E190" s="7">
+      <c r="E196" s="7">
         <v>0.78</v>
       </c>
-      <c r="F190" s="7">
+      <c r="F196" s="7">
         <f>0.0055*10^4</f>
         <v>55</v>
       </c>
-      <c r="G190" s="7">
+      <c r="G196" s="7">
         <v>2.7</v>
       </c>
-      <c r="H190" s="7">
+      <c r="H196" s="7">
         <v>3</v>
       </c>
-      <c r="I190" s="7">
+      <c r="I196" s="7">
         <v>0.2</v>
       </c>
-      <c r="J190" s="5">
+      <c r="J196" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A191" s="6" t="s">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A197" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B191" s="7">
+      <c r="B197" s="7">
         <v>140</v>
       </c>
-      <c r="C191" s="7">
+      <c r="C197" s="7">
         <v>6.2</v>
       </c>
-      <c r="D191" s="7">
+      <c r="D197" s="7">
         <v>2.8</v>
       </c>
-      <c r="E191" s="7">
+      <c r="E197" s="7">
         <v>0.53</v>
       </c>
-      <c r="F191" s="7">
+      <c r="F197" s="7">
         <v>85</v>
       </c>
-      <c r="G191" s="7">
+      <c r="G197" s="7">
         <v>1.45</v>
       </c>
-      <c r="H191" s="7">
+      <c r="H197" s="7">
         <v>3</v>
       </c>
-      <c r="I191" s="7">
+      <c r="I197" s="7">
         <v>0.2</v>
       </c>
-      <c r="J191" s="5">
+      <c r="J197" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A192" s="6" t="s">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A198" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B192" s="7">
+      <c r="B198" s="7">
         <v>63</v>
       </c>
-      <c r="C192" s="7">
+      <c r="C198" s="7">
         <v>5.3</v>
       </c>
-      <c r="D192" s="7">
+      <c r="D198" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E192" s="7">
+      <c r="E198" s="7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F192" s="7">
+      <c r="F198" s="7">
         <v>85</v>
       </c>
-      <c r="G192" s="7">
+      <c r="G198" s="7">
         <v>5.8</v>
       </c>
-      <c r="H192" s="7">
+      <c r="H198" s="7">
         <v>5.5</v>
       </c>
-      <c r="I192" s="7">
+      <c r="I198" s="7">
         <v>0.2</v>
       </c>
-      <c r="J192" s="5">
+      <c r="J198" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A193" s="6" t="s">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A199" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B193" s="7">
+      <c r="B199" s="7">
         <v>72</v>
       </c>
-      <c r="C193" s="7">
+      <c r="C199" s="7">
         <v>5.2</v>
       </c>
-      <c r="D193" s="7">
+      <c r="D199" s="7">
         <v>7.5</v>
       </c>
-      <c r="E193" s="7">
+      <c r="E199" s="7">
         <v>0.35</v>
       </c>
-      <c r="F193" s="7">
+      <c r="F199" s="7">
         <v>95</v>
       </c>
-      <c r="G193" s="7">
+      <c r="G199" s="7">
         <v>5.69</v>
       </c>
-      <c r="H193" s="7">
+      <c r="H199" s="7">
         <v>5.7</v>
       </c>
-      <c r="I193" s="7">
+      <c r="I199" s="7">
         <v>0.6</v>
       </c>
-      <c r="J193" s="5">
+      <c r="J199" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A194" s="6" t="s">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A200" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B194" s="7">
+      <c r="B200" s="7">
         <v>78</v>
       </c>
-      <c r="C194" s="7">
+      <c r="C200" s="7">
         <v>5.3</v>
       </c>
-      <c r="D194" s="7">
+      <c r="D200" s="7">
         <v>10.7</v>
       </c>
-      <c r="E194" s="7">
+      <c r="E200" s="7">
         <v>0.31</v>
       </c>
-      <c r="F194" s="7">
+      <c r="F200" s="7">
         <v>95</v>
       </c>
-      <c r="G194" s="7">
+      <c r="G200" s="7">
         <v>4.5</v>
       </c>
-      <c r="H194" s="7">
+      <c r="H200" s="7">
         <v>5.7</v>
       </c>
-      <c r="I194" s="7">
+      <c r="I200" s="7">
         <v>0.3</v>
       </c>
-      <c r="J194" s="5">
+      <c r="J200" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A195" s="6" t="s">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A201" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B201" s="7">
+        <v>150</v>
+      </c>
+      <c r="C201" s="7">
+        <v>6</v>
+      </c>
+      <c r="D201" s="7">
+        <v>9.68</v>
+      </c>
+      <c r="E201" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="F201" s="7">
+        <v>140</v>
+      </c>
+      <c r="G201" s="7">
+        <v>3</v>
+      </c>
+      <c r="H201" s="7">
+        <v>1</v>
+      </c>
+      <c r="I201" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J201" s="5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A202" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B195" s="7">
+      <c r="B202" s="7">
         <v>56</v>
       </c>
-      <c r="C195" s="7">
+      <c r="C202" s="7">
         <v>5.5</v>
       </c>
-      <c r="D195" s="7">
+      <c r="D202" s="7">
         <v>3</v>
       </c>
-      <c r="E195" s="7">
+      <c r="E202" s="7">
         <v>0.6</v>
       </c>
-      <c r="F195" s="7">
+      <c r="F202" s="7">
         <f>0.014*10^4</f>
         <v>140</v>
       </c>
-      <c r="G195" s="7">
+      <c r="G202" s="7">
         <v>15.6</v>
       </c>
-      <c r="H195" s="7">
+      <c r="H202" s="7">
         <v>5.5</v>
       </c>
-      <c r="I195" s="7">
+      <c r="I202" s="7">
         <v>0.3</v>
       </c>
-      <c r="J195" s="5">
+      <c r="J202" s="5">
         <v>40</v>
-      </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A196" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B196" s="7">
-        <v>90</v>
-      </c>
-      <c r="C196" s="7">
-        <v>5.3</v>
-      </c>
-      <c r="D196" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="E196" s="7">
-        <v>0.45</v>
-      </c>
-      <c r="F196" s="7">
-        <v>140</v>
-      </c>
-      <c r="G196" s="7">
-        <v>6.5</v>
-      </c>
-      <c r="H196" s="7">
-        <v>5.7</v>
-      </c>
-      <c r="I196" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="J196" s="5">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A197" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B197" s="7">
-        <v>102</v>
-      </c>
-      <c r="C197" s="7">
-        <v>6</v>
-      </c>
-      <c r="D197" s="7">
-        <v>9.25</v>
-      </c>
-      <c r="E197" s="7">
-        <v>0.42</v>
-      </c>
-      <c r="F197" s="7">
-        <v>140</v>
-      </c>
-      <c r="G197" s="7">
-        <v>5.04</v>
-      </c>
-      <c r="H197" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="I197" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="J197" s="5">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A198" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B198" s="7">
-        <v>85</v>
-      </c>
-      <c r="C198" s="7">
-        <v>6</v>
-      </c>
-      <c r="D198" s="7">
-        <v>3.7</v>
-      </c>
-      <c r="E198" s="7">
-        <v>0.36</v>
-      </c>
-      <c r="F198" s="7">
-        <v>140</v>
-      </c>
-      <c r="G198" s="7">
-        <v>7</v>
-      </c>
-      <c r="H198" s="7">
-        <v>3</v>
-      </c>
-      <c r="I198" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="J198" s="5">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A199" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B199" s="7">
-        <v>406</v>
-      </c>
-      <c r="C199" s="7">
-        <v>6.2</v>
-      </c>
-      <c r="D199" s="7">
-        <v>10.3</v>
-      </c>
-      <c r="E199" s="7">
-        <v>0.77</v>
-      </c>
-      <c r="F199" s="7">
-        <v>140</v>
-      </c>
-      <c r="G199" s="7">
-        <v>0.27</v>
-      </c>
-      <c r="H199" s="7">
-        <v>2.5</v>
-      </c>
-      <c r="I199" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="J199" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A200" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B200" s="7">
-        <v>58</v>
-      </c>
-      <c r="C200" s="7">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D200" s="7">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E200" s="7">
-        <v>0.27</v>
-      </c>
-      <c r="F200" s="7">
-        <v>135</v>
-      </c>
-      <c r="G200" s="7">
-        <v>11.1</v>
-      </c>
-      <c r="H200" s="7">
-        <v>5.5</v>
-      </c>
-      <c r="I200" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="J200" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A201" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B201" s="7">
-        <v>52</v>
-      </c>
-      <c r="C201" s="7">
-        <v>5.5</v>
-      </c>
-      <c r="D201" s="7">
-        <v>5.56</v>
-      </c>
-      <c r="E201" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F201" s="7">
-        <v>220</v>
-      </c>
-      <c r="G201" s="7">
-        <v>29.6</v>
-      </c>
-      <c r="H201" s="7">
-        <v>5.7</v>
-      </c>
-      <c r="I201" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="J201" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A202" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B202" s="7">
-        <v>30</v>
-      </c>
-      <c r="C202" s="7">
-        <v>5.5</v>
-      </c>
-      <c r="D202" s="7">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="E202" s="7">
-        <v>0.48</v>
-      </c>
-      <c r="F202" s="7">
-        <v>220</v>
-      </c>
-      <c r="G202" s="7">
-        <v>89.1</v>
-      </c>
-      <c r="H202" s="7">
-        <v>6.7</v>
-      </c>
-      <c r="I202" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="J202" s="5">
-        <v>50</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A203" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B203" s="7">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C203" s="7">
-        <v>5.0999999999999996</v>
+        <v>5.3</v>
       </c>
       <c r="D203" s="7">
-        <v>7.7</v>
+        <v>1.4</v>
       </c>
       <c r="E203" s="7">
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
       <c r="F203" s="7">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="G203" s="7">
-        <v>14.6</v>
+        <v>6.5</v>
       </c>
       <c r="H203" s="7">
         <v>5.7</v>
       </c>
       <c r="I203" s="7">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="J203" s="5">
-        <v>250</v>
+        <v>220</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A204" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B204" s="7">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="C204" s="7">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="D204" s="7">
-        <v>6.83</v>
+        <v>9.25</v>
       </c>
       <c r="E204" s="7">
-        <v>0.38</v>
+        <v>0.42</v>
       </c>
       <c r="F204" s="7">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="G204" s="7">
-        <v>17</v>
+        <v>5.04</v>
       </c>
       <c r="H204" s="7">
-        <v>4.5</v>
+        <v>3.1</v>
       </c>
       <c r="I204" s="7">
-        <v>1.3</v>
+        <v>0.5</v>
       </c>
       <c r="J204" s="5">
-        <v>250</v>
+        <v>170</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A205" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B205" s="7">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C205" s="7">
-        <v>6.2</v>
+        <v>6</v>
       </c>
       <c r="D205" s="7">
-        <v>6.2</v>
+        <v>3.7</v>
       </c>
       <c r="E205" s="7">
-        <v>0.28999999999999998</v>
+        <v>0.36</v>
       </c>
       <c r="F205" s="7">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="G205" s="7">
-        <v>11.6</v>
+        <v>7</v>
       </c>
       <c r="H205" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I205" s="7">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="J205" s="5">
-        <v>300</v>
+        <v>170</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A206" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B206" s="7">
-        <v>75</v>
+        <v>406</v>
       </c>
       <c r="C206" s="7">
-        <v>5.3</v>
+        <v>6.2</v>
       </c>
       <c r="D206" s="7">
-        <v>3</v>
+        <v>10.3</v>
       </c>
       <c r="E206" s="7">
-        <v>0.2</v>
+        <v>0.77</v>
       </c>
       <c r="F206" s="7">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="G206" s="7">
-        <v>12.2</v>
+        <v>0.27</v>
       </c>
       <c r="H206" s="7">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="I206" s="7">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J206" s="5">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A207" s="6" t="s">
-        <v>51</v>
+        <v>249</v>
       </c>
       <c r="B207" s="7">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="C207" s="7">
         <v>6</v>
       </c>
       <c r="D207" s="7">
-        <v>7.5</v>
+        <v>8.6</v>
       </c>
       <c r="E207" s="7">
-        <v>0.48</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F207" s="7">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="G207" s="7">
-        <v>12</v>
+        <v>3.07</v>
       </c>
       <c r="H207" s="7">
         <v>3</v>
@@ -8540,417 +8579,690 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A208" s="6" t="s">
-        <v>52</v>
+        <v>250</v>
       </c>
       <c r="B208" s="7">
-        <v>53</v>
+        <v>134</v>
       </c>
       <c r="C208" s="7">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="D208" s="7">
-        <v>14.3</v>
+        <v>8.4</v>
       </c>
       <c r="E208" s="7">
-        <v>0.32</v>
+        <v>0.44</v>
       </c>
       <c r="F208" s="7">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="G208" s="7">
-        <v>24.8</v>
+        <v>3.35</v>
       </c>
       <c r="H208" s="7">
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="I208" s="7">
         <v>0.4</v>
       </c>
       <c r="J208" s="5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A209" s="6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B209" s="7">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C209" s="7">
-        <v>5.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D209" s="7">
-        <v>2.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E209" s="7">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="F209" s="7">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="G209" s="7">
-        <v>17.7</v>
+        <v>11.1</v>
       </c>
       <c r="H209" s="7">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="I209" s="7">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="J209" s="5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A210" s="6" t="s">
-        <v>54</v>
+        <v>251</v>
       </c>
       <c r="B210" s="7">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C210" s="7">
-        <v>5.9</v>
+        <v>5.3</v>
       </c>
       <c r="D210" s="7">
-        <v>2.7</v>
+        <v>3.69</v>
       </c>
       <c r="E210" s="7">
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
       <c r="F210" s="7">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="G210" s="7">
-        <v>13.1</v>
+        <v>11.9</v>
       </c>
       <c r="H210" s="7">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="I210" s="7">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="J210" s="5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A211" s="6" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="B211" s="7">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C211" s="7">
-        <v>6.2</v>
+        <v>5.5</v>
       </c>
       <c r="D211" s="7">
-        <v>3.8</v>
+        <v>5.56</v>
       </c>
       <c r="E211" s="7">
-        <v>0.35</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F211" s="7">
         <v>220</v>
       </c>
       <c r="G211" s="7">
-        <v>14.4</v>
+        <v>29.6</v>
       </c>
       <c r="H211" s="7">
-        <v>6</v>
+        <v>5.7</v>
       </c>
       <c r="I211" s="7">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="J211" s="5">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A212" s="6" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="B212" s="7">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C212" s="7">
-        <v>6.2</v>
+        <v>5.5</v>
       </c>
       <c r="D212" s="7">
-        <v>7.88</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="E212" s="7">
-        <v>0.37</v>
+        <v>0.48</v>
       </c>
       <c r="F212" s="7">
-        <v>355</v>
+        <v>220</v>
       </c>
       <c r="G212" s="7">
-        <v>65</v>
+        <v>89.1</v>
       </c>
       <c r="H212" s="7">
-        <v>4</v>
+        <v>6.7</v>
       </c>
       <c r="I212" s="7">
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="J212" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A213" s="6" t="s">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="B213" s="7">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C213" s="7">
         <v>6.2</v>
       </c>
       <c r="D213" s="7">
-        <v>8</v>
+        <v>13.46</v>
       </c>
       <c r="E213" s="7">
-        <v>0.31</v>
+        <v>0.65</v>
       </c>
       <c r="F213" s="7">
-        <v>550</v>
+        <v>220</v>
       </c>
       <c r="G213" s="7">
-        <v>117.3</v>
+        <v>14.6</v>
       </c>
       <c r="H213" s="7">
-        <v>7.25</v>
+        <v>6.7</v>
       </c>
       <c r="I213" s="7">
         <v>1.2</v>
       </c>
       <c r="J213" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A214" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B214" s="7">
+        <v>75</v>
+      </c>
+      <c r="C214" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D214" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="E214" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F214" s="7">
+        <v>220</v>
+      </c>
+      <c r="G214" s="7">
+        <v>14.6</v>
+      </c>
+      <c r="H214" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="I214" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="J214" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A215" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B215" s="7">
+        <v>70</v>
+      </c>
+      <c r="C215" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="D215" s="7">
+        <v>6.83</v>
+      </c>
+      <c r="E215" s="7">
+        <v>0.38</v>
+      </c>
+      <c r="F215" s="7">
+        <v>220</v>
+      </c>
+      <c r="G215" s="7">
+        <v>17</v>
+      </c>
+      <c r="H215" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="I215" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="J215" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A216" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B216" s="7">
+        <v>70</v>
+      </c>
+      <c r="C216" s="7">
+        <v>5.8</v>
+      </c>
+      <c r="D216" s="7">
+        <v>7</v>
+      </c>
+      <c r="E216" s="7">
+        <v>0.39</v>
+      </c>
+      <c r="F216" s="7">
+        <v>220</v>
+      </c>
+      <c r="G216" s="7">
+        <v>16</v>
+      </c>
+      <c r="H216" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="I216" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J216" s="5">
+        <v>250</v>
+      </c>
+      <c r="L216" s="7"/>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A217" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B217" s="7">
+        <v>76</v>
+      </c>
+      <c r="C217" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="D217" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="E217" s="7">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F217" s="7">
+        <v>220</v>
+      </c>
+      <c r="G217" s="7">
+        <v>11.6</v>
+      </c>
+      <c r="H217" s="7">
+        <v>6</v>
+      </c>
+      <c r="I217" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J217" s="5">
+        <v>300</v>
+      </c>
+      <c r="L217" s="7"/>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A218" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B218" s="7">
+        <v>75</v>
+      </c>
+      <c r="C218" s="7">
+        <v>5.3</v>
+      </c>
+      <c r="D218" s="7">
+        <v>3</v>
+      </c>
+      <c r="E218" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F218" s="7">
+        <v>220</v>
+      </c>
+      <c r="G218" s="7">
+        <v>12.2</v>
+      </c>
+      <c r="H218" s="7">
+        <v>5</v>
+      </c>
+      <c r="I218" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J218" s="5">
+        <v>500</v>
+      </c>
+      <c r="L218" s="7"/>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A219" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B219" s="7">
+        <v>90</v>
+      </c>
+      <c r="C219" s="7">
+        <v>6</v>
+      </c>
+      <c r="D219" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="E219" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="F219" s="7">
+        <v>220</v>
+      </c>
+      <c r="G219" s="7">
+        <v>12</v>
+      </c>
+      <c r="H219" s="7">
+        <v>3</v>
+      </c>
+      <c r="I219" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="J219" s="5">
+        <v>250</v>
+      </c>
+      <c r="L219" s="7"/>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A220" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B220" s="7">
+        <v>53</v>
+      </c>
+      <c r="C220" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="D220" s="7">
+        <v>14.3</v>
+      </c>
+      <c r="E220" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="F220" s="7">
+        <v>220</v>
+      </c>
+      <c r="G220" s="7">
+        <v>24.8</v>
+      </c>
+      <c r="H220" s="7">
+        <v>6</v>
+      </c>
+      <c r="I220" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="J220" s="5">
+        <v>300</v>
+      </c>
+      <c r="L220" s="7"/>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A221" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B221" s="7">
+        <v>35</v>
+      </c>
+      <c r="C221" s="7">
+        <v>5.8</v>
+      </c>
+      <c r="D221" s="7">
+        <v>2.72</v>
+      </c>
+      <c r="E221" s="7">
+        <v>0.62</v>
+      </c>
+      <c r="F221" s="7">
+        <v>220</v>
+      </c>
+      <c r="G221" s="7">
+        <v>59</v>
+      </c>
+      <c r="H221" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="I221" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J221" s="5">
+        <v>50</v>
+      </c>
+      <c r="L221" s="7"/>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A222" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B222" s="7">
+        <v>62</v>
+      </c>
+      <c r="C222" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="D222" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="E222" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="F222" s="7">
+        <v>220</v>
+      </c>
+      <c r="G222" s="7">
+        <v>17.7</v>
+      </c>
+      <c r="H222" s="7">
+        <v>6</v>
+      </c>
+      <c r="I222" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J222" s="5">
+        <v>300</v>
+      </c>
+      <c r="L222" s="7"/>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A223" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B223" s="7">
+        <v>69</v>
+      </c>
+      <c r="C223" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="D223" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="E223" s="7">
+        <v>0.34</v>
+      </c>
+      <c r="F223" s="7">
+        <v>220</v>
+      </c>
+      <c r="G223" s="7">
+        <v>13.1</v>
+      </c>
+      <c r="H223" s="7">
+        <v>6</v>
+      </c>
+      <c r="I223" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J223" s="5">
+        <v>300</v>
+      </c>
+      <c r="L223" s="7"/>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A224" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B224" s="7">
+        <v>71</v>
+      </c>
+      <c r="C224" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="D224" s="7">
+        <v>3.8</v>
+      </c>
+      <c r="E224" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="F224" s="7">
+        <v>220</v>
+      </c>
+      <c r="G224" s="7">
+        <v>14.4</v>
+      </c>
+      <c r="H224" s="7">
+        <v>6</v>
+      </c>
+      <c r="I224" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J224" s="5">
+        <v>150</v>
+      </c>
+      <c r="L224" s="7"/>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A225" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B225" s="7">
+        <v>43</v>
+      </c>
+      <c r="C225" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="D225" s="7">
+        <v>7.88</v>
+      </c>
+      <c r="E225" s="7">
+        <v>0.37</v>
+      </c>
+      <c r="F225" s="7">
+        <v>355</v>
+      </c>
+      <c r="G225" s="7">
+        <v>65</v>
+      </c>
+      <c r="H225" s="7">
+        <v>4</v>
+      </c>
+      <c r="I225" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="J225" s="5">
+        <v>200</v>
+      </c>
+      <c r="L225" s="7"/>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A226" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B226" s="7">
+        <v>40</v>
+      </c>
+      <c r="C226" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="D226" s="7">
+        <v>8</v>
+      </c>
+      <c r="E226" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="F226" s="7">
+        <v>550</v>
+      </c>
+      <c r="G226" s="7">
+        <v>117.3</v>
+      </c>
+      <c r="H226" s="7">
+        <v>7.25</v>
+      </c>
+      <c r="I226" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="J226" s="5">
         <v>400</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A214" s="6" t="s">
+      <c r="L226" s="7"/>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A227" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B214" s="7">
+      <c r="B227" s="7">
         <v>29</v>
       </c>
-      <c r="C214" s="7">
+      <c r="C227" s="7">
         <v>6.1</v>
       </c>
-      <c r="D214" s="7">
+      <c r="D227" s="7">
         <v>5.8</v>
       </c>
-      <c r="E214" s="7">
+      <c r="E227" s="7">
         <v>0.26</v>
       </c>
-      <c r="F214" s="7">
+      <c r="F227" s="7">
         <v>880</v>
       </c>
-      <c r="G214" s="7">
+      <c r="G227" s="7">
         <v>273</v>
       </c>
-      <c r="H214" s="7">
+      <c r="H227" s="7">
         <v>8</v>
       </c>
-      <c r="I214" s="7">
+      <c r="I227" s="7">
         <v>1.6</v>
       </c>
-      <c r="J214" s="5">
+      <c r="J227" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A215" s="6" t="s">
+      <c r="L227" s="7"/>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A228" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B215" s="7">
+      <c r="B228" s="7">
         <v>43</v>
       </c>
-      <c r="C215" s="7">
+      <c r="C228" s="7">
         <v>5.5</v>
       </c>
-      <c r="D215" s="7">
+      <c r="D228" s="7">
         <v>5.3</v>
       </c>
-      <c r="E215" s="7">
+      <c r="E228" s="7">
         <v>0.41</v>
       </c>
-      <c r="F215" s="7">
+      <c r="F228" s="7">
         <v>550</v>
       </c>
-      <c r="G215" s="7">
+      <c r="G228" s="7">
         <v>103</v>
       </c>
-      <c r="H215" s="7">
+      <c r="H228" s="7">
         <v>8.25</v>
       </c>
-      <c r="I215" s="7">
+      <c r="I228" s="7">
         <v>0.6</v>
       </c>
-      <c r="J215" s="5">
+      <c r="J228" s="5">
         <v>350</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A216" s="6"/>
-      <c r="B216" s="7"/>
-      <c r="C216" s="7"/>
-      <c r="D216" s="7"/>
-      <c r="E216" s="7"/>
-      <c r="F216" s="7"/>
-      <c r="G216" s="7"/>
-      <c r="H216" s="7"/>
-      <c r="I216" s="7"/>
-      <c r="J216" s="7"/>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A217" s="6"/>
-      <c r="B217" s="7"/>
-      <c r="C217" s="7"/>
-      <c r="D217" s="7"/>
-      <c r="E217" s="7"/>
-      <c r="F217" s="7"/>
-      <c r="G217" s="7"/>
-      <c r="H217" s="7"/>
-      <c r="I217" s="7"/>
-      <c r="J217" s="7"/>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A218" s="6"/>
-      <c r="B218" s="7"/>
-      <c r="C218" s="7"/>
-      <c r="D218" s="7"/>
-      <c r="E218" s="7"/>
-      <c r="F218" s="7"/>
-      <c r="G218" s="7"/>
-      <c r="H218" s="7"/>
-      <c r="I218" s="7"/>
-      <c r="J218" s="7"/>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A219" s="6"/>
-      <c r="B219" s="7"/>
-      <c r="C219" s="7"/>
-      <c r="D219" s="7"/>
-      <c r="E219" s="7"/>
-      <c r="F219" s="7"/>
-      <c r="G219" s="7"/>
-      <c r="H219" s="7"/>
-      <c r="I219" s="7"/>
-      <c r="J219" s="7"/>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A220" s="6"/>
-      <c r="B220" s="7"/>
-      <c r="C220" s="7"/>
-      <c r="D220" s="7"/>
-      <c r="E220" s="7"/>
-      <c r="F220" s="7"/>
-      <c r="G220" s="7"/>
-      <c r="H220" s="7"/>
-      <c r="I220" s="7"/>
-      <c r="J220" s="7"/>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A221" s="6"/>
-      <c r="B221" s="7"/>
-      <c r="C221" s="7"/>
-      <c r="D221" s="7"/>
-      <c r="E221" s="7"/>
-      <c r="F221" s="7"/>
-      <c r="G221" s="7"/>
-      <c r="H221" s="7"/>
-      <c r="I221" s="7"/>
-      <c r="J221" s="7"/>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A222" s="6"/>
-      <c r="B222" s="7"/>
-      <c r="C222" s="7"/>
-      <c r="D222" s="7"/>
-      <c r="E222" s="7"/>
-      <c r="F222" s="7"/>
-      <c r="G222" s="7"/>
-      <c r="H222" s="7"/>
-      <c r="I222" s="7"/>
-      <c r="J222" s="7"/>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A223" s="6"/>
-      <c r="B223" s="7"/>
-      <c r="C223" s="7"/>
-      <c r="D223" s="7"/>
-      <c r="E223" s="7"/>
-      <c r="F223" s="7"/>
-      <c r="G223" s="7"/>
-      <c r="H223" s="7"/>
-      <c r="I223" s="7"/>
-      <c r="J223" s="7"/>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A224" s="6"/>
-      <c r="B224" s="7"/>
-      <c r="C224" s="7"/>
-      <c r="D224" s="7"/>
-      <c r="E224" s="7"/>
-      <c r="F224" s="7"/>
-      <c r="G224" s="7"/>
-      <c r="H224" s="7"/>
-      <c r="I224" s="7"/>
-      <c r="J224" s="7"/>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A225" s="6"/>
-      <c r="B225" s="7"/>
-      <c r="C225" s="7"/>
-      <c r="D225" s="7"/>
-      <c r="E225" s="7"/>
-      <c r="F225" s="7"/>
-      <c r="G225" s="7"/>
-      <c r="H225" s="7"/>
-      <c r="I225" s="7"/>
-      <c r="J225" s="7"/>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A226" s="6"/>
-      <c r="B226" s="7"/>
-      <c r="C226" s="7"/>
-      <c r="D226" s="7"/>
-      <c r="E226" s="7"/>
-      <c r="F226" s="7"/>
-      <c r="G226" s="7"/>
-      <c r="H226" s="7"/>
-      <c r="I226" s="7"/>
-      <c r="J226" s="7"/>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A227" s="6"/>
-      <c r="B227" s="7"/>
-      <c r="C227" s="7"/>
-      <c r="D227" s="7"/>
-      <c r="E227" s="7"/>
-      <c r="F227" s="7"/>
-      <c r="G227" s="7"/>
-      <c r="H227" s="7"/>
-      <c r="I227" s="7"/>
-      <c r="J227" s="7"/>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A228" s="6"/>
-      <c r="B228" s="7"/>
-      <c r="C228" s="7"/>
-      <c r="D228" s="7"/>
-      <c r="E228" s="7"/>
-      <c r="F228" s="7"/>
-      <c r="G228" s="7"/>
-      <c r="H228" s="7"/>
-      <c r="I228" s="7"/>
-      <c r="J228" s="7"/>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="L228" s="7"/>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A229" s="6"/>
       <c r="B229" s="7"/>
       <c r="C229" s="7"/>
@@ -8962,7 +9274,7 @@
       <c r="I229" s="7"/>
       <c r="J229" s="7"/>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A230" s="6"/>
       <c r="B230" s="7"/>
       <c r="C230" s="7"/>
@@ -8974,7 +9286,7 @@
       <c r="I230" s="7"/>
       <c r="J230" s="7"/>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A231" s="6"/>
       <c r="B231" s="7"/>
       <c r="C231" s="7"/>
@@ -8986,7 +9298,7 @@
       <c r="I231" s="7"/>
       <c r="J231" s="7"/>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A232" s="6"/>
       <c r="B232" s="7"/>
       <c r="C232" s="7"/>
@@ -8998,7 +9310,7 @@
       <c r="I232" s="7"/>
       <c r="J232" s="7"/>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A233" s="6"/>
       <c r="B233" s="7"/>
       <c r="C233" s="7"/>
@@ -9010,7 +9322,7 @@
       <c r="I233" s="7"/>
       <c r="J233" s="7"/>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A234" s="6"/>
       <c r="B234" s="7"/>
       <c r="C234" s="7"/>
@@ -9022,7 +9334,7 @@
       <c r="I234" s="7"/>
       <c r="J234" s="7"/>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A235" s="6"/>
       <c r="B235" s="7"/>
       <c r="C235" s="7"/>
@@ -9034,7 +9346,7 @@
       <c r="I235" s="7"/>
       <c r="J235" s="7"/>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A236" s="6"/>
       <c r="B236" s="7"/>
       <c r="C236" s="7"/>
@@ -9046,7 +9358,7 @@
       <c r="I236" s="7"/>
       <c r="J236" s="7"/>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A237" s="6"/>
       <c r="B237" s="7"/>
       <c r="C237" s="7"/>
@@ -9058,7 +9370,7 @@
       <c r="I237" s="7"/>
       <c r="J237" s="7"/>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A238" s="6"/>
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
@@ -9070,7 +9382,7 @@
       <c r="I238" s="7"/>
       <c r="J238" s="7"/>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A239" s="6"/>
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
@@ -9082,7 +9394,7 @@
       <c r="I239" s="7"/>
       <c r="J239" s="7"/>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A240" s="6"/>
       <c r="B240" s="7"/>
       <c r="C240" s="7"/>
@@ -12130,8 +12442,8 @@
       <c r="J493" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J215">
-    <sortCondition ref="A4:A215"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J228">
+    <sortCondition ref="A4:A228"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{AEE76D55-8BA2-104C-A7C3-D743A1275482}">

</xml_diff>